<commit_message>
11-5-2019 Final Documentation Updates
</commit_message>
<xml_diff>
--- a/prj/hazelnut_large/LHC-001/1-Documentation/LHC-300 Light Assembly Fabrication Checklist - ONGOING.xlsx
+++ b/prj/hazelnut_large/LHC-001/1-Documentation/LHC-300 Light Assembly Fabrication Checklist - ONGOING.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Open AG\Documents\GitHub\openag-mechanical\prj\hazelnut_large\LHC-001\1-Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugen\Documents\GitHub\openag-mechanical\prj\hazelnut_large\LHC-001\1-Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA57D71-8FBB-432B-8A8F-D4EEF5AE3878}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B733F8-0FA6-482B-83DC-D182ED5C4A6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{C1DC14C7-5C89-45DF-BE4F-6E1CF3C084B8}"/>
+    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{C1DC14C7-5C89-45DF-BE4F-6E1CF3C084B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -929,29 +929,29 @@
   </sheetPr>
   <dimension ref="A1:BK65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" customWidth="1"/>
-    <col min="4" max="4" width="11.90625" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" customWidth="1"/>
-    <col min="7" max="7" width="9.90625" customWidth="1"/>
-    <col min="8" max="8" width="8.453125" customWidth="1"/>
-    <col min="9" max="9" width="36.453125" customWidth="1"/>
-    <col min="10" max="10" width="13.453125" customWidth="1"/>
-    <col min="11" max="11" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="18" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="34" width="5.81640625" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" customWidth="1"/>
+    <col min="9" max="9" width="36.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="18" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="34" width="5.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:63" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1054,7 +1054,7 @@
       <c r="BJ1" s="28"/>
       <c r="BK1" s="28"/>
     </row>
-    <row r="2" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -1142,7 +1142,7 @@
       <c r="BJ2" s="29"/>
       <c r="BK2" s="29"/>
     </row>
-    <row r="3" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1223,7 +1223,7 @@
       <c r="BJ3" s="2"/>
       <c r="BK3" s="2"/>
     </row>
-    <row r="4" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -1304,7 +1304,7 @@
       <c r="BJ4" s="2"/>
       <c r="BK4" s="2"/>
     </row>
-    <row r="5" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1385,7 +1385,7 @@
       <c r="BJ5" s="2"/>
       <c r="BK5" s="2"/>
     </row>
-    <row r="6" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -1466,7 +1466,7 @@
       <c r="BJ6" s="2"/>
       <c r="BK6" s="2"/>
     </row>
-    <row r="7" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -1547,7 +1547,7 @@
       <c r="BJ7" s="2"/>
       <c r="BK7" s="2"/>
     </row>
-    <row r="8" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1628,7 +1628,7 @@
       <c r="BJ8" s="2"/>
       <c r="BK8" s="2"/>
     </row>
-    <row r="9" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
@@ -1709,7 +1709,7 @@
       <c r="BJ9" s="2"/>
       <c r="BK9" s="2"/>
     </row>
-    <row r="10" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -1790,7 +1790,7 @@
       <c r="BJ10" s="2"/>
       <c r="BK10" s="2"/>
     </row>
-    <row r="11" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -1871,7 +1871,7 @@
       <c r="BJ11" s="2"/>
       <c r="BK11" s="2"/>
     </row>
-    <row r="12" spans="1:63" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:63" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
@@ -1969,7 +1969,7 @@
       <c r="BJ12" s="2"/>
       <c r="BK12" s="2"/>
     </row>
-    <row r="13" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -2050,7 +2050,7 @@
       <c r="BJ13" s="2"/>
       <c r="BK13" s="2"/>
     </row>
-    <row r="14" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
@@ -2131,7 +2131,7 @@
       <c r="BJ14" s="2"/>
       <c r="BK14" s="2"/>
     </row>
-    <row r="15" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -2212,7 +2212,7 @@
       <c r="BJ15" s="2"/>
       <c r="BK15" s="2"/>
     </row>
-    <row r="16" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
@@ -2293,7 +2293,7 @@
       <c r="BJ16" s="2"/>
       <c r="BK16" s="2"/>
     </row>
-    <row r="17" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>16</v>
       </c>
@@ -2374,7 +2374,7 @@
       <c r="BJ17" s="2"/>
       <c r="BK17" s="2"/>
     </row>
-    <row r="18" spans="1:63" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:63" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -2472,7 +2472,7 @@
       <c r="BJ18" s="2"/>
       <c r="BK18" s="2"/>
     </row>
-    <row r="19" spans="1:63" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:63" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
@@ -2570,7 +2570,7 @@
       <c r="BJ19" s="2"/>
       <c r="BK19" s="2"/>
     </row>
-    <row r="20" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -2651,7 +2651,7 @@
       <c r="BJ20" s="2"/>
       <c r="BK20" s="2"/>
     </row>
-    <row r="21" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>20</v>
       </c>
@@ -2732,7 +2732,7 @@
       <c r="BJ21" s="2"/>
       <c r="BK21" s="2"/>
     </row>
-    <row r="22" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>21</v>
       </c>
@@ -2813,7 +2813,7 @@
       <c r="BJ22" s="2"/>
       <c r="BK22" s="2"/>
     </row>
-    <row r="23" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -2894,7 +2894,7 @@
       <c r="BJ23" s="2"/>
       <c r="BK23" s="2"/>
     </row>
-    <row r="24" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>23</v>
       </c>
@@ -2975,7 +2975,7 @@
       <c r="BJ24" s="2"/>
       <c r="BK24" s="2"/>
     </row>
-    <row r="25" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -3056,7 +3056,7 @@
       <c r="BJ25" s="2"/>
       <c r="BK25" s="2"/>
     </row>
-    <row r="26" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>25</v>
       </c>
@@ -3144,7 +3144,7 @@
       <c r="BJ26" s="2"/>
       <c r="BK26" s="2"/>
     </row>
-    <row r="27" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>26</v>
       </c>
@@ -3225,7 +3225,7 @@
       <c r="BJ27" s="2"/>
       <c r="BK27" s="2"/>
     </row>
-    <row r="28" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -3306,7 +3306,7 @@
       <c r="BJ28" s="2"/>
       <c r="BK28" s="2"/>
     </row>
-    <row r="29" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>28</v>
       </c>
@@ -3387,7 +3387,7 @@
       <c r="BJ29" s="2"/>
       <c r="BK29" s="2"/>
     </row>
-    <row r="30" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
@@ -3468,7 +3468,7 @@
       <c r="BJ30" s="2"/>
       <c r="BK30" s="2"/>
     </row>
-    <row r="31" spans="1:63" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:63" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="14" t="s">
         <v>30</v>
       </c>
@@ -3549,7 +3549,7 @@
       <c r="BJ31" s="2"/>
       <c r="BK31" s="2"/>
     </row>
-    <row r="32" spans="1:63" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:63" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J32" s="24"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
@@ -3605,7 +3605,7 @@
       <c r="BJ32" s="2"/>
       <c r="BK32" s="2"/>
     </row>
-    <row r="33" spans="1:63" ht="61" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:63" ht="60.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
         <v>0</v>
       </c>
@@ -3688,7 +3688,7 @@
       <c r="BJ33" s="2"/>
       <c r="BK33" s="2"/>
     </row>
-    <row r="34" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>31</v>
       </c>
@@ -3769,7 +3769,7 @@
       <c r="BJ34" s="2"/>
       <c r="BK34" s="2"/>
     </row>
-    <row r="35" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>32</v>
       </c>
@@ -3850,7 +3850,7 @@
       <c r="BJ35" s="2"/>
       <c r="BK35" s="2"/>
     </row>
-    <row r="36" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>33</v>
       </c>
@@ -3933,7 +3933,7 @@
       <c r="BJ36" s="2"/>
       <c r="BK36" s="2"/>
     </row>
-    <row r="37" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>34</v>
       </c>
@@ -4014,7 +4014,7 @@
       <c r="BJ37" s="2"/>
       <c r="BK37" s="2"/>
     </row>
-    <row r="38" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>35</v>
       </c>
@@ -4095,7 +4095,7 @@
       <c r="BJ38" s="2"/>
       <c r="BK38" s="2"/>
     </row>
-    <row r="39" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>36</v>
       </c>
@@ -4176,7 +4176,7 @@
       <c r="BJ39" s="2"/>
       <c r="BK39" s="2"/>
     </row>
-    <row r="40" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>37</v>
       </c>
@@ -4264,7 +4264,7 @@
       <c r="BJ40" s="2"/>
       <c r="BK40" s="2"/>
     </row>
-    <row r="41" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>38</v>
       </c>
@@ -4345,7 +4345,7 @@
       <c r="BJ41" s="2"/>
       <c r="BK41" s="2"/>
     </row>
-    <row r="42" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>39</v>
       </c>
@@ -4426,7 +4426,7 @@
       <c r="BJ42" s="2"/>
       <c r="BK42" s="2"/>
     </row>
-    <row r="43" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>40</v>
       </c>
@@ -4507,7 +4507,7 @@
       <c r="BJ43" s="2"/>
       <c r="BK43" s="2"/>
     </row>
-    <row r="44" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>41</v>
       </c>
@@ -4588,7 +4588,7 @@
       <c r="BJ44" s="2"/>
       <c r="BK44" s="2"/>
     </row>
-    <row r="45" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>42</v>
       </c>
@@ -4669,7 +4669,7 @@
       <c r="BJ45" s="2"/>
       <c r="BK45" s="2"/>
     </row>
-    <row r="46" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>43</v>
       </c>
@@ -4750,7 +4750,7 @@
       <c r="BJ46" s="2"/>
       <c r="BK46" s="2"/>
     </row>
-    <row r="47" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>44</v>
       </c>
@@ -4831,7 +4831,7 @@
       <c r="BJ47" s="2"/>
       <c r="BK47" s="2"/>
     </row>
-    <row r="48" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>45</v>
       </c>
@@ -4912,7 +4912,7 @@
       <c r="BJ48" s="2"/>
       <c r="BK48" s="2"/>
     </row>
-    <row r="49" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>46</v>
       </c>
@@ -4993,7 +4993,7 @@
       <c r="BJ49" s="2"/>
       <c r="BK49" s="2"/>
     </row>
-    <row r="50" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>47</v>
       </c>
@@ -5074,7 +5074,7 @@
       <c r="BJ50" s="2"/>
       <c r="BK50" s="2"/>
     </row>
-    <row r="51" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>48</v>
       </c>
@@ -5155,7 +5155,7 @@
       <c r="BJ51" s="2"/>
       <c r="BK51" s="2"/>
     </row>
-    <row r="52" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>49</v>
       </c>
@@ -5169,7 +5169,7 @@
       <c r="I52" s="4"/>
       <c r="J52" s="24"/>
     </row>
-    <row r="53" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>50</v>
       </c>
@@ -5183,7 +5183,7 @@
       <c r="I53" s="4"/>
       <c r="J53" s="24"/>
     </row>
-    <row r="54" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>51</v>
       </c>
@@ -5197,7 +5197,7 @@
       <c r="I54" s="4"/>
       <c r="J54" s="24"/>
     </row>
-    <row r="55" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>52</v>
       </c>
@@ -5211,7 +5211,7 @@
       <c r="I55" s="4"/>
       <c r="J55" s="24"/>
     </row>
-    <row r="56" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>53</v>
       </c>
@@ -5225,7 +5225,7 @@
       <c r="I56" s="4"/>
       <c r="J56" s="24"/>
     </row>
-    <row r="57" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>54</v>
       </c>
@@ -5239,7 +5239,7 @@
       <c r="I57" s="4"/>
       <c r="J57" s="24"/>
     </row>
-    <row r="58" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>55</v>
       </c>
@@ -5253,7 +5253,7 @@
       <c r="I58" s="4"/>
       <c r="J58" s="24"/>
     </row>
-    <row r="59" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>56</v>
       </c>
@@ -5267,7 +5267,7 @@
       <c r="I59" s="4"/>
       <c r="J59" s="24"/>
     </row>
-    <row r="60" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
         <v>57</v>
       </c>
@@ -5281,7 +5281,7 @@
       <c r="I60" s="4"/>
       <c r="J60" s="24"/>
     </row>
-    <row r="61" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>58</v>
       </c>
@@ -5295,7 +5295,7 @@
       <c r="I61" s="4"/>
       <c r="J61" s="24"/>
     </row>
-    <row r="62" spans="1:63" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
         <v>59</v>
       </c>
@@ -5309,7 +5309,7 @@
       <c r="I62" s="4"/>
       <c r="J62" s="24"/>
     </row>
-    <row r="63" spans="1:63" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:63" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>60</v>
       </c>
@@ -5323,10 +5323,10 @@
       <c r="I63" s="6"/>
       <c r="J63" s="24"/>
     </row>
-    <row r="64" spans="1:63" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:63" ht="18.75" x14ac:dyDescent="0.3">
       <c r="J64" s="25"/>
     </row>
-    <row r="65" spans="10:10" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="65" spans="10:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="J65" s="25"/>
     </row>
   </sheetData>

</xml_diff>